<commit_message>
Feat: Add final EDA notebook and professional folder structure
</commit_message>
<xml_diff>
--- a/data/raw/equipment_costs.xlsx
+++ b/data/raw/equipment_costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snehalsahu/Downloads/work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasob\Downloads\EV_Diesel_Project\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002B87C7-180D-7345-B880-B898769B1954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288AEFE7-F8B8-40F2-B1C3-4A5CBD06FDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{D57857AB-9A8A-A542-AE05-A81876355AD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D57857AB-9A8A-A542-AE05-A81876355AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1625,16 +1625,16 @@
   <dimension ref="A1:I241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="16.296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="5" width="16.33203125" style="90"/>
-    <col min="8" max="8" width="16.33203125" style="64"/>
+    <col min="4" max="5" width="16.296875" style="90"/>
+    <col min="8" max="8" width="16.296875" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>106</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>4561551880</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>132</v>
       </c>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>104</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>4561551879</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>14</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>14</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>85</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>85</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>4097001795</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>44</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>4561551513</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>40</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>4561549950</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>144</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>4097002414</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>146</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>4097001801</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>144</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>4097001984</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>29</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>4097002136</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>29</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>4561552718</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>54</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>4561550968</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>21</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>4561551460</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>67</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>4561551460</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="46" t="s">
         <v>206</v>
       </c>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="46" t="s">
         <v>206</v>
       </c>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>266</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>78</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>4561548927</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>170</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="74"/>
     </row>
-    <row r="31" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35" t="s">
         <v>93</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>235000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
         <v>93</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>235000</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>264</v>
       </c>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>69</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>4561552697</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>69</v>
       </c>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="H35" s="25"/>
     </row>
-    <row r="36" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>69</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>4561549555</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>69</v>
       </c>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="H37" s="25"/>
     </row>
-    <row r="38" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
         <v>69</v>
       </c>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="H38" s="25"/>
     </row>
-    <row r="39" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>69</v>
       </c>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="49" t="s">
         <v>69</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>69</v>
       </c>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>69</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>4561552978</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="37" t="s">
         <v>69</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>4561552612</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="37" t="s">
         <v>69</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>4561545909</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="37" t="s">
         <v>69</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>4561552610</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="40" t="s">
         <v>110</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>4561552907</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
         <v>108</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>4561552906</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>45</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>4561549345</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>45</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>4561547726</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>45</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>4561547728</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>45</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>4561547754</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="40" t="s">
         <v>112</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>4561550514</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
         <v>194</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>140</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>142</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>8</v>
       </c>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="42" t="s">
         <v>117</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>4561552322</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="42" t="s">
         <v>117</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>4561552323</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="44" t="s">
         <v>128</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>4561552327</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="42" t="s">
         <v>125</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>4561552668</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="42" t="s">
         <v>125</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>4561552325</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="42" t="s">
         <v>125</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>4561552326</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="44" t="s">
         <v>120</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>4561548149</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>21</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>21</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>21</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="22" t="s">
         <v>71</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18" t="s">
         <v>21</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="46" t="s">
         <v>21</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
         <v>23</v>
       </c>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="H70" s="26"/>
     </row>
-    <row r="71" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="24" t="s">
         <v>67</v>
       </c>
@@ -3481,7 +3481,7 @@
       </c>
       <c r="H71" s="26"/>
     </row>
-    <row r="72" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
         <v>69</v>
       </c>
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H72" s="26"/>
     </row>
-    <row r="73" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>67</v>
       </c>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="H73" s="13"/>
     </row>
-    <row r="74" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>69</v>
       </c>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="H74" s="13"/>
     </row>
-    <row r="75" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="29" t="s">
         <v>21</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>166</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>155000</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>135</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>56</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18" t="s">
         <v>67</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
         <v>67</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>330000</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>67</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>330000</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
         <v>67</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
         <v>67</v>
       </c>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H83" s="13"/>
     </row>
-    <row r="84" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
         <v>23</v>
       </c>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="H84" s="13"/>
     </row>
-    <row r="85" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
         <v>189</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>330000</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>67</v>
       </c>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H86" s="13"/>
     </row>
-    <row r="87" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
         <v>174</v>
       </c>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="H87" s="13"/>
     </row>
-    <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="24" t="s">
         <v>189</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
         <v>174</v>
       </c>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H89" s="13"/>
     </row>
-    <row r="90" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="24" t="s">
         <v>189</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>330000</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="29" t="s">
         <v>67</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="29" t="s">
         <v>67</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>660000</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="29" t="s">
         <v>67</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>660000</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="18" t="s">
         <v>67</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>4561551923</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="11" t="s">
         <v>67</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>660000</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="11" t="s">
         <v>59</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="11" t="s">
         <v>59</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>7260000</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="11" t="s">
         <v>42</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="11" t="s">
         <v>36</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>215000</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>144</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="24" t="s">
         <v>21</v>
       </c>
@@ -4292,7 +4292,7 @@
       </c>
       <c r="H101" s="13"/>
     </row>
-    <row r="102" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="24" t="s">
         <v>17</v>
       </c>
@@ -4312,7 +4312,7 @@
       </c>
       <c r="H102" s="13"/>
     </row>
-    <row r="103" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="24" t="s">
         <v>14</v>
       </c>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="H103" s="13"/>
     </row>
-    <row r="104" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>174</v>
       </c>
@@ -4352,7 +4352,7 @@
       </c>
       <c r="H104" s="13"/>
     </row>
-    <row r="105" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="11" t="s">
         <v>63</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="18" t="s">
         <v>63</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>17</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="24" t="s">
         <v>17</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="11" t="s">
         <v>17</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="11" t="s">
         <v>17</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="18" t="s">
         <v>17</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="24" t="s">
         <v>17</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="24" t="s">
         <v>17</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="24" t="s">
         <v>17</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="46" t="s">
         <v>17</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="29" t="s">
         <v>17</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="29" t="s">
         <v>17</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="39" t="s">
         <v>17</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="46" t="s">
         <v>67</v>
       </c>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="H119" s="13"/>
     </row>
-    <row r="120" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="46" t="s">
         <v>23</v>
       </c>
@@ -4790,7 +4790,7 @@
       </c>
       <c r="H120" s="13"/>
     </row>
-    <row r="121" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="46" t="s">
         <v>201</v>
       </c>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="H121" s="13"/>
     </row>
-    <row r="122" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="46" t="s">
         <v>202</v>
       </c>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="H122" s="13"/>
     </row>
-    <row r="123" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="46" t="s">
         <v>137</v>
       </c>
@@ -4862,7 +4862,7 @@
       </c>
       <c r="H123" s="13"/>
     </row>
-    <row r="124" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="46" t="s">
         <v>205</v>
       </c>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="H124" s="13"/>
     </row>
-    <row r="125" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="46" t="s">
         <v>137</v>
       </c>
@@ -4910,7 +4910,7 @@
       </c>
       <c r="H125" s="13"/>
     </row>
-    <row r="126" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="11" t="s">
         <v>17</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="11" t="s">
         <v>153</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>105000</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="11" t="s">
         <v>267</v>
       </c>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="H128" s="13"/>
     </row>
-    <row r="129" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="46" t="s">
         <v>21</v>
       </c>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="H129" s="13"/>
     </row>
-    <row r="130" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="46" t="s">
         <v>213</v>
       </c>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="H130" s="13"/>
     </row>
-    <row r="131" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="46" t="s">
         <v>214</v>
       </c>
@@ -5050,7 +5050,7 @@
       </c>
       <c r="H131" s="13"/>
     </row>
-    <row r="132" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>23</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="24" t="s">
         <v>23</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="46" t="s">
         <v>23</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="37" t="s">
         <v>23</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="46" t="s">
         <v>209</v>
       </c>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="H136" s="13"/>
     </row>
-    <row r="137" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="18" t="s">
         <v>65</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>4097003433</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="24" t="s">
         <v>82</v>
       </c>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="H138" s="13"/>
     </row>
-    <row r="139" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="33" t="s">
         <v>82</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>4561552286</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>27</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>4097002348</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="22" t="s">
         <v>155</v>
       </c>
@@ -5315,7 +5315,7 @@
       </c>
       <c r="I141" s="73"/>
     </row>
-    <row r="142" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="11" t="s">
         <v>47</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="29" t="s">
         <v>174</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="29" t="s">
         <v>174</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="17" t="s">
         <v>151</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="29" t="s">
         <v>216</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>4563503824</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="17" t="s">
         <v>152</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>4561551519</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="29" t="s">
         <v>217</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>4563503824</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="29" t="s">
         <v>215</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>4563503649</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>24</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>4097003586</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="29" t="s">
         <v>24</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>4563504024</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="55" t="s">
         <v>67</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>4561549729</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="55" t="s">
         <v>220</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>4561549729</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="55" t="s">
         <v>67</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>4561549893</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="55" t="s">
         <v>220</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>4561549893</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="55" t="s">
         <v>69</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>4561544800</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>19</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>4097003705</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="29" t="s">
         <v>19</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>4563503649</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="46" t="s">
         <v>199</v>
       </c>
@@ -5791,7 +5791,7 @@
       </c>
       <c r="H159" s="13"/>
     </row>
-    <row r="160" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="24" t="s">
         <v>182</v>
       </c>
@@ -5815,7 +5815,7 @@
       </c>
       <c r="H160" s="13"/>
     </row>
-    <row r="161" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="57" t="s">
         <v>221</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>4561547528</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="57" t="s">
         <v>17</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>4561552589</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="57" t="s">
         <v>85</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>4561552589</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="57" t="s">
         <v>71</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>4561552589</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="57" t="s">
         <v>224</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>4561552589</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="11" t="s">
         <v>29</v>
       </c>
@@ -5947,7 +5947,7 @@
       </c>
       <c r="H166" s="13"/>
     </row>
-    <row r="167" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>225</v>
       </c>
@@ -5971,7 +5971,7 @@
       </c>
       <c r="H167" s="54"/>
     </row>
-    <row r="168" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>225</v>
       </c>
@@ -5995,7 +5995,7 @@
       </c>
       <c r="H168" s="13"/>
     </row>
-    <row r="169" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="17" t="s">
         <v>34</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>4561551519</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="11" t="s">
         <v>57</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>4561551619</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="20" t="s">
         <v>180</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>145000</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="22" t="s">
         <v>115</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>145000</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="20" t="s">
         <v>154</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>145000</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="11" t="s">
         <v>38</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>145000</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="18" t="s">
         <v>177</v>
       </c>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="H175" s="13"/>
     </row>
-    <row r="176" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="46" t="s">
         <v>198</v>
       </c>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="H176" s="13"/>
     </row>
-    <row r="177" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>12</v>
       </c>
@@ -6233,7 +6233,7 @@
       </c>
       <c r="H177" s="4"/>
     </row>
-    <row r="178" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="18" t="s">
         <v>12</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>4561551265</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="20" t="s">
         <v>62</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>4561552648</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="24" t="s">
         <v>62</v>
       </c>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H180" s="25"/>
     </row>
-    <row r="181" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="24" t="s">
         <v>62</v>
       </c>
@@ -6333,7 +6333,7 @@
       </c>
       <c r="H181" s="25"/>
     </row>
-    <row r="182" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="24" t="s">
         <v>62</v>
       </c>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="H182" s="25"/>
     </row>
-    <row r="183" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="11" t="s">
         <v>12</v>
       </c>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="H183" s="13"/>
     </row>
-    <row r="184" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="40" t="s">
         <v>240</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>4561549552</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="15" t="s">
         <v>242</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="15" t="s">
         <v>243</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="15" t="s">
         <v>244</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="15" t="s">
         <v>245</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="15" t="s">
         <v>246</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="15" t="s">
         <v>247</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="15" t="s">
         <v>248</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="15" t="s">
         <v>249</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="15" t="s">
         <v>250</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="15" t="s">
         <v>251</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>4561552590</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="22" t="s">
         <v>137</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>4563503939</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="22" t="s">
         <v>69</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>4563503488</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="22" t="s">
         <v>67</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>4563503488</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="11" t="s">
         <v>62</v>
       </c>
@@ -6769,7 +6769,7 @@
       </c>
       <c r="H198" s="65"/>
     </row>
-    <row r="199" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="29" t="s">
         <v>252</v>
       </c>
@@ -6793,7 +6793,7 @@
       </c>
       <c r="H199" s="13"/>
     </row>
-    <row r="200" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="29" t="s">
         <v>254</v>
       </c>
@@ -6817,7 +6817,7 @@
       </c>
       <c r="H200" s="13"/>
     </row>
-    <row r="201" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="22" t="s">
         <v>137</v>
       </c>
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H201" s="13"/>
     </row>
-    <row r="202" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="11" t="s">
         <v>174</v>
       </c>
@@ -6857,7 +6857,7 @@
       <c r="G202" s="13"/>
       <c r="H202" s="13"/>
     </row>
-    <row r="203" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="11" t="s">
         <v>17</v>
       </c>
@@ -6873,7 +6873,7 @@
       <c r="G203" s="13"/>
       <c r="H203" s="13"/>
     </row>
-    <row r="204" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="11" t="s">
         <v>14</v>
       </c>
@@ -6889,7 +6889,7 @@
       <c r="G204" s="13"/>
       <c r="H204" s="13"/>
     </row>
-    <row r="205" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="11" t="s">
         <v>67</v>
       </c>
@@ -6909,7 +6909,7 @@
       </c>
       <c r="H205" s="13"/>
     </row>
-    <row r="206" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="11" t="s">
         <v>67</v>
       </c>
@@ -6929,7 +6929,7 @@
       </c>
       <c r="H206" s="13"/>
     </row>
-    <row r="207" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="11" t="s">
         <v>258</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>4561545493</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="11" t="s">
         <v>23</v>
       </c>
@@ -6971,7 +6971,7 @@
       <c r="G208" s="13"/>
       <c r="H208" s="13"/>
     </row>
-    <row r="209" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="11" t="s">
         <v>69</v>
       </c>
@@ -6987,7 +6987,7 @@
       <c r="G209" s="13"/>
       <c r="H209" s="13"/>
     </row>
-    <row r="210" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="11" t="s">
         <v>67</v>
       </c>
@@ -7003,7 +7003,7 @@
       <c r="G210" s="13"/>
       <c r="H210" s="13"/>
     </row>
-    <row r="211" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="11" t="s">
         <v>261</v>
       </c>
@@ -7019,7 +7019,7 @@
       <c r="G211" s="13"/>
       <c r="H211" s="13"/>
     </row>
-    <row r="212" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="11" t="s">
         <v>262</v>
       </c>
@@ -7035,7 +7035,7 @@
       <c r="G212" s="13"/>
       <c r="H212" s="13"/>
     </row>
-    <row r="213" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="24" t="s">
         <v>12</v>
       </c>
@@ -7059,7 +7059,7 @@
       </c>
       <c r="H213" s="13"/>
     </row>
-    <row r="214" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="11" t="s">
         <v>12</v>
       </c>
@@ -7083,7 +7083,7 @@
       </c>
       <c r="H214" s="13"/>
     </row>
-    <row r="215" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="11" t="s">
         <v>12</v>
       </c>
@@ -7107,7 +7107,7 @@
       </c>
       <c r="H215" s="13"/>
     </row>
-    <row r="216" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="11" t="s">
         <v>12</v>
       </c>
@@ -7131,7 +7131,7 @@
       </c>
       <c r="H216" s="13"/>
     </row>
-    <row r="217" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="11" t="s">
         <v>12</v>
       </c>
@@ -7155,7 +7155,7 @@
       </c>
       <c r="H217" s="13"/>
     </row>
-    <row r="218" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="11" t="s">
         <v>237</v>
       </c>
@@ -7179,7 +7179,7 @@
       </c>
       <c r="H218" s="13"/>
     </row>
-    <row r="219" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="11" t="s">
         <v>50</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>4561547603</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>137</v>
       </c>
@@ -7229,7 +7229,7 @@
       </c>
       <c r="H220" s="4"/>
     </row>
-    <row r="221" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>137</v>
       </c>
@@ -7253,7 +7253,7 @@
       </c>
       <c r="H221" s="7"/>
     </row>
-    <row r="222" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="11" t="s">
         <v>60</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>4561547862</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="39" t="s">
         <v>102</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>4561546708</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="44" t="s">
         <v>122</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>4561546314</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="44" t="s">
         <v>122</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>4561552753</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="44" t="s">
         <v>130</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>4561552137</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="44" t="s">
         <v>130</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>4561552136</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="44" t="s">
         <v>130</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>4561552138</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="61" t="s">
         <v>268</v>
       </c>
@@ -7459,7 +7459,7 @@
       </c>
       <c r="H229" s="63"/>
     </row>
-    <row r="230" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="61" t="s">
         <v>271</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="61" t="s">
         <v>272</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="61" t="s">
         <v>273</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="61" t="s">
         <v>274</v>
       </c>
@@ -7551,7 +7551,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="61" t="s">
         <v>275</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="61" t="s">
         <v>276</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="61" t="s">
         <v>153</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="61" t="s">
         <v>277</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="61" t="s">
         <v>278</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="61" t="s">
         <v>279</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="61" t="s">
         <v>280</v>
       </c>
@@ -7712,7 +7712,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="61" t="s">
         <v>281</v>
       </c>
@@ -7765,7 +7765,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>